<commit_message>
Added diagrams and updated BOM
</commit_message>
<xml_diff>
--- a/documentation/BOM.xlsx
+++ b/documentation/BOM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{173432DF-F54B-4967-B1B0-E4B38990C9D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4963687-5983-4324-9B15-75CFD2D3B9F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>Description</t>
   </si>
@@ -103,13 +103,37 @@
   </si>
   <si>
     <t>CF14JT100R</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>AC/DC WALL MOUNT ADAPTER 9V 5W</t>
+  </si>
+  <si>
+    <t>VEL05US090-US-JA</t>
+  </si>
+  <si>
+    <t>BUMPER SQU 0.812"L X 0.812"W BLK</t>
+  </si>
+  <si>
+    <t>SJ-5523 (BLACK)</t>
+  </si>
+  <si>
+    <t>USB CABLE TYPE A TO B 30CM BLACK</t>
+  </si>
+  <si>
+    <t>Seeed Technology Co., Ltd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +152,21 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -171,23 +210,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -466,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G13"/>
+  <dimension ref="B2:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,109 +557,115 @@
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="4">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4">
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5">
         <v>20.9</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="5">
+        <f>E3*D3</f>
         <v>20.9</v>
       </c>
-      <c r="G3" s="4"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <v>103030215</v>
       </c>
-      <c r="D4" s="4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="4">
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5">
         <v>24.99</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="5">
+        <f t="shared" ref="F4:F9" si="0">E4*D4</f>
         <v>24.99</v>
       </c>
-      <c r="G4" s="4"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="4">
-        <v>1</v>
-      </c>
-      <c r="E5" s="4">
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5">
         <v>0.39</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="5">
+        <f t="shared" si="0"/>
         <v>0.39</v>
       </c>
-      <c r="G5" s="4"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="4">
-        <v>1</v>
-      </c>
-      <c r="E6" s="4">
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5">
         <v>0.39</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="5">
+        <f t="shared" si="0"/>
         <v>0.39</v>
       </c>
-      <c r="G6" s="4"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="4">
-        <v>1</v>
-      </c>
-      <c r="E7" s="4">
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5">
         <v>1.38</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="5">
+        <f t="shared" si="0"/>
         <v>1.38</v>
       </c>
-      <c r="G7" s="4"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="4">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4">
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5">
         <v>4.3499999999999996</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="5">
+        <f t="shared" si="0"/>
         <v>4.3499999999999996</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -616,19 +673,20 @@
       <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="4">
-        <v>1</v>
-      </c>
-      <c r="E9" s="4">
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5">
         <v>0.63</v>
       </c>
-      <c r="F9" s="4">
-        <v>1.26</v>
-      </c>
-      <c r="G9" s="4" t="s">
+      <c r="F9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.63</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -636,19 +694,19 @@
       <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="4">
         <v>73412</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>4</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -656,19 +714,19 @@
       <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="4">
         <v>71004</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>4</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -676,19 +734,19 @@
       <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="4">
         <v>1170704</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>4</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -696,20 +754,93 @@
       <c r="B13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="4">
-        <v>1</v>
-      </c>
-      <c r="E13" s="4">
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+      <c r="E13" s="5">
         <v>0.1</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="5">
+        <f>E13*D13</f>
         <v>0.1</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="3" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="6">
+        <v>6.5</v>
+      </c>
+      <c r="F14" s="5">
+        <f t="shared" ref="F14:F16" si="1">E14*D14</f>
+        <v>6.5</v>
+      </c>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+      <c r="E15" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="F15" s="5">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16" s="6">
+        <v>1.99</v>
+      </c>
+      <c r="F16" s="5">
+        <f t="shared" si="1"/>
+        <v>1.99</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="7">
+        <f>SUM(F3:F16)</f>
+        <v>63.120000000000012</v>
       </c>
     </row>
   </sheetData>

</xml_diff>